<commit_message>
Added keyword (HK of fgDG)
</commit_message>
<xml_diff>
--- a/JSON/fgDeGender_Trefwoorden.xlsx
+++ b/JSON/fgDeGender_Trefwoorden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808A1E60-B5EF-4747-8647-A1ACCB611A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2481FF18-208D-6947-B946-3D46C94FC7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26440" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="72">
   <si>
     <t>Albert</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t xml:space="preserve">    ‣ Je mag een ontbrekend trefwoord voorstellen (vaak leverbaar ;-)</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -427,6 +430,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -435,12 +444,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,7 +1244,7 @@
   <autoFilter ref="A6:T30" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
   <tableColumns count="20">
     <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="19">
-      <totalsRowFormula>COUNTA(A7:A30)/COUNTA(B7:B30)</totalsRowFormula>
+      <totalsRowFormula>COUNTA(A7:A29)/COUNTA(B7:B29)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="38" totalsRowDxfId="18"/>
     <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="37" totalsRowDxfId="17"/>
@@ -1620,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB03C53-D149-8D47-9F9C-2A5FA6F563CA}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -1643,65 +1646,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="T1" s="19">
         <v>45774</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
     </row>
     <row r="6" spans="1:20" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1766,7 +1769,9 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="B7" s="13" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1803,9 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="B8" s="13" t="s">
         <v>18</v>
       </c>
@@ -2001,8 +2008,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="52" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+    <row r="14" spans="1:20" ht="58" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="B14" s="13" t="s">
         <v>27</v>
       </c>
@@ -2011,7 +2020,9 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="F14" s="22" t="s">
+        <v>11</v>
+      </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -2032,7 +2043,7 @@
       <c r="T14" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
@@ -2136,7 +2147,9 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
+      <c r="A18" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="B18" s="13" t="s">
         <v>39</v>
       </c>
@@ -2308,7 +2321,7 @@
         <v>51</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="10"/>
@@ -2561,55 +2574,55 @@
       <c r="T30" s="12"/>
     </row>
     <row r="31" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24">
-        <f>COUNTA(A7:A30)/COUNTA(B7:B30)</f>
-        <v>0.34782608695652173</v>
+      <c r="A31" s="21">
+        <f>COUNTA(A7:A29)/COUNTA(B7:B29)</f>
+        <v>0.52173913043478259</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E31" s="16">
-        <f>COUNTA(E7:E30)</f>
+        <f t="shared" ref="E31:N31" si="0">COUNTA(E7:E30)</f>
         <v>1</v>
       </c>
       <c r="F31" s="16">
-        <f>COUNTA(F7:F30)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="G31" s="16">
-        <f>COUNTA(G7:G30)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H31" s="16">
-        <f>COUNTA(H7:H30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I31" s="16">
-        <f>COUNTA(I7:I30)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J31" s="16">
-        <f>COUNTA(J7:J30)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K31" s="16">
-        <f>COUNTA(K7:K30)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L31" s="16">
-        <f>COUNTA(L7:L30)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="M31" s="16">
-        <f>COUNTA(M7:M30)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N31" s="16">
-        <f>COUNTA(N7:N30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O31" s="16">
-        <f t="shared" ref="E31:S31" si="0">COUNTA(O7:O30)</f>
+        <f t="shared" ref="O31" si="1">COUNTA(O7:O30)</f>
         <v>4</v>
       </c>
       <c r="P31" s="16">
@@ -2630,7 +2643,7 @@
       </c>
       <c r="T31" s="18">
         <f>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</f>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new Museum keyword Keywords for AK of fgDG
</commit_message>
<xml_diff>
--- a/JSON/fgDeGender_Trefwoorden.xlsx
+++ b/JSON/fgDeGender_Trefwoorden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2481FF18-208D-6947-B946-3D46C94FC7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6F36B5-198D-9747-AA0B-EDCE5C4B087C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26440" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Albert</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Museum</t>
   </si>
 </sst>
 </file>
@@ -376,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -445,11 +448,17 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="45">
     <dxf>
       <font>
         <b val="0"/>
@@ -752,6 +761,24 @@
         <sz val="16"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
@@ -809,6 +836,24 @@
       </font>
       <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1240,61 +1285,64 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:T31" totalsRowCount="1" headerRowDxfId="42" dataDxfId="41" totalsRowDxfId="40">
-  <autoFilter ref="A6:T30" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
-  <tableColumns count="20">
-    <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:U31" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43" totalsRowDxfId="42">
+  <autoFilter ref="A6:U30" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
+  <tableColumns count="21">
+    <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="20">
       <totalsRowFormula>COUNTA(A7:A29)/COUNTA(B7:B29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="38" totalsRowDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="37" totalsRowDxfId="17"/>
-    <tableColumn id="18" xr3:uid="{F762D242-8B7F-1147-BBFB-3246F5000811}" name="eventueel voorstel voor _x000a_nieuw trefwoord" totalsRowLabel="#" dataDxfId="36" totalsRowDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{3B6A13EE-99F5-7441-8057-E1A06F70075A}" name="Abstract" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="15">
+    <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="40" totalsRowDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="39" totalsRowDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{F762D242-8B7F-1147-BBFB-3246F5000811}" name="eventueel voorstel voor _x000a_nieuw trefwoord" totalsRowLabel="#" dataDxfId="38" totalsRowDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{3B6A13EE-99F5-7441-8057-E1A06F70075A}" name="Abstract" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="16">
       <totalsRowFormula>COUNTA(E7:E30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E9B92604-5273-624A-92B0-22FFB11BEC40}" name="Architectuur" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="14">
+    <tableColumn id="4" xr3:uid="{E9B92604-5273-624A-92B0-22FFB11BEC40}" name="Architectuur" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="15">
       <totalsRowFormula>COUNTA(F7:F30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{832AF978-DCE3-DA47-B36A-9D928FCF0BF1}" name="Conceptueel" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="13">
+    <tableColumn id="6" xr3:uid="{832AF978-DCE3-DA47-B36A-9D928FCF0BF1}" name="Conceptueel" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="14">
       <totalsRowFormula>COUNTA(G7:G30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64143930-3345-DA4D-9135-20E16BCCB08E}" name="Concert" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="12">
+    <tableColumn id="7" xr3:uid="{64143930-3345-DA4D-9135-20E16BCCB08E}" name="Concert" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="13">
       <totalsRowFormula>COUNTA(H7:H30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="11">
+    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="12">
       <totalsRowFormula>COUNTA(I7:I30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="10">
+    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="11">
       <totalsRowFormula>COUNTA(J7:J30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="9">
+    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="10">
       <totalsRowFormula>COUNTA(K7:K30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="8">
+    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="9">
       <totalsRowFormula>COUNTA(L7:L30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="7">
+    <tableColumn id="5" xr3:uid="{34A8085A-25B7-B64C-9185-7DCD6F2A68CF}" name="Museum" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="8">
       <totalsRowFormula>COUNTA(M7:M30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="6">
+    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="7">
       <totalsRowFormula>COUNTA(N7:N30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="5">
+    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="6">
       <totalsRowFormula>COUNTA(O7:O30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="4">
+    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="5">
       <totalsRowFormula>COUNTA(P7:P30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="3">
+    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="4">
       <totalsRowFormula>COUNTA(Q7:Q30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="2">
+    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="3">
       <totalsRowFormula>COUNTA(R7:R30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="1">
+    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="2">
       <totalsRowFormula>COUNTA(S7:S30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="0">
+    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="1">
+      <totalsRowFormula>COUNTA(T7:T30)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="0">
       <calculatedColumnFormula>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</totalsRowFormula>
@@ -1621,10 +1669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB03C53-D149-8D47-9F9C-2A5FA6F563CA}">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -1637,15 +1685,15 @@
     <col min="6" max="6" width="10.83203125" style="1"/>
     <col min="7" max="10" width="10.83203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="14" width="10.83203125" style="1" customWidth="1"/>
-    <col min="15" max="17" width="10.83203125" style="1"/>
-    <col min="18" max="18" width="13.83203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" style="1"/>
-    <col min="20" max="20" width="11.5" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="1"/>
+    <col min="12" max="15" width="10.83203125" style="1" customWidth="1"/>
+    <col min="16" max="18" width="10.83203125" style="1"/>
+    <col min="19" max="19" width="13.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" style="1"/>
+    <col min="21" max="21" width="11.5" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>67</v>
       </c>
@@ -1655,11 +1703,11 @@
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
-      <c r="T1" s="19">
+      <c r="U1" s="19">
         <v>45774</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="25" t="s">
         <v>69</v>
@@ -1668,7 +1716,7 @@
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25" t="s">
         <v>70</v>
@@ -1677,7 +1725,7 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="24"/>
       <c r="B4" s="25" t="s">
         <v>68</v>
@@ -1686,7 +1734,7 @@
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -1705,8 +1753,9 @@
       <c r="P5" s="23"/>
       <c r="Q5" s="23"/>
       <c r="R5" s="23"/>
-    </row>
-    <row r="6" spans="1:20" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="S5" s="23"/>
+    </row>
+    <row r="6" spans="1:21" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
@@ -1743,34 +1792,37 @@
       <c r="L6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="Q6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="R6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="S6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="T6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="U6" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>71</v>
+    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>0</v>
@@ -1787,22 +1839,27 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="M7" s="27" t="s">
+        <v>72</v>
+      </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="R7" s="10"/>
       <c r="S7" s="10"/>
-      <c r="T7" s="12">
+      <c r="T7" s="10"/>
+      <c r="U7" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>71</v>
       </c>
@@ -1828,13 +1885,14 @@
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
-      <c r="T8" s="12">
+      <c r="T8" s="10"/>
+      <c r="U8" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="38" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
         <v>20</v>
@@ -1856,17 +1914,18 @@
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
-      <c r="R9" s="9" t="s">
+      <c r="R9" s="10"/>
+      <c r="S9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S9" s="10"/>
-      <c r="T9" s="12">
+      <c r="T9" s="10"/>
+      <c r="U9" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="55" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="55" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>63</v>
       </c>
@@ -1889,22 +1948,23 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="9" t="s">
+      <c r="O10" s="10"/>
+      <c r="P10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="Q10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="12">
+      <c r="T10" s="10"/>
+      <c r="U10" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="65" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="65" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
         <v>23</v>
@@ -1923,22 +1983,23 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="9" t="s">
+      <c r="M11" s="10"/>
+      <c r="N11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="10"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="9"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="12">
+      <c r="T11" s="10"/>
+      <c r="U11" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="39" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>63</v>
       </c>
@@ -1961,22 +2022,23 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="9" t="s">
+      <c r="O12" s="10"/>
+      <c r="P12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="Q12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
-      <c r="T12" s="12">
+      <c r="T12" s="10"/>
+      <c r="U12" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
         <v>27</v>
@@ -2002,13 +2064,14 @@
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="12">
+      <c r="T13" s="10"/>
+      <c r="U13" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="58" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="58" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>63</v>
       </c>
@@ -2037,16 +2100,17 @@
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
-      <c r="S14" s="9" t="s">
+      <c r="S14" s="10"/>
+      <c r="T14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="T14" s="12">
+      <c r="U14" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="13" t="s">
         <v>33</v>
@@ -2070,13 +2134,14 @@
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="12">
+      <c r="T15" s="10"/>
+      <c r="U15" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="47" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="13" t="s">
         <v>35</v>
@@ -2095,20 +2160,21 @@
       <c r="L16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="10"/>
+      <c r="M16" s="9"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
-      <c r="T16" s="12">
+      <c r="T16" s="10"/>
+      <c r="U16" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="65" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="65" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>63</v>
       </c>
@@ -2132,21 +2198,22 @@
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="9" t="s">
+      <c r="N17" s="10"/>
+      <c r="O17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O17" s="10"/>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
-      <c r="T17" s="12">
+      <c r="T17" s="10"/>
+      <c r="U17" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>71</v>
       </c>
@@ -2172,13 +2239,14 @@
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
-      <c r="T18" s="12">
+      <c r="T18" s="10"/>
+      <c r="U18" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="13" t="s">
         <v>42</v>
@@ -2202,13 +2270,14 @@
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="12">
+      <c r="T19" s="10"/>
+      <c r="U19" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="52" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="52" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
@@ -2231,22 +2300,23 @@
       <c r="L20" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M20" s="10"/>
+      <c r="M20" s="9"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
-      <c r="Q20" s="9" t="s">
+      <c r="Q20" s="10"/>
+      <c r="R20" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="R20" s="10"/>
       <c r="S20" s="10"/>
-      <c r="T20" s="12">
+      <c r="T20" s="10"/>
+      <c r="U20" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="65" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="65" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="13" t="s">
         <v>46</v>
@@ -2272,13 +2342,14 @@
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="12">
+      <c r="T21" s="10"/>
+      <c r="U21" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="52" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="52" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="s">
         <v>48</v>
@@ -2304,13 +2375,14 @@
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
-      <c r="T22" s="12">
+      <c r="T22" s="10"/>
+      <c r="U22" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="65" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="65" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>63</v>
       </c>
@@ -2335,20 +2407,21 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="9"/>
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
-      <c r="T23" s="12">
+      <c r="T23" s="10"/>
+      <c r="U23" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="60" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="60" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>63</v>
       </c>
@@ -2371,22 +2444,23 @@
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="9" t="s">
+      <c r="M24" s="10"/>
+      <c r="N24" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N24" s="10"/>
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
-      <c r="T24" s="12">
+      <c r="T24" s="10"/>
+      <c r="U24" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="13" t="s">
         <v>54</v>
@@ -2410,13 +2484,14 @@
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
-      <c r="T25" s="12">
+      <c r="T25" s="10"/>
+      <c r="U25" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
       <c r="B26" s="13" t="s">
         <v>56</v>
@@ -2437,18 +2512,19 @@
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
-      <c r="Q26" s="9" t="s">
+      <c r="Q26" s="10"/>
+      <c r="R26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="R26" s="10"/>
       <c r="S26" s="10"/>
-      <c r="T26" s="12">
+      <c r="T26" s="10"/>
+      <c r="U26" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>63</v>
       </c>
@@ -2469,20 +2545,21 @@
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
-      <c r="O27" s="9" t="s">
+      <c r="O27" s="10"/>
+      <c r="P27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
-      <c r="T27" s="12">
+      <c r="T27" s="10"/>
+      <c r="U27" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="38" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="38" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="13" t="s">
         <v>60</v>
@@ -2504,17 +2581,18 @@
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
-      <c r="R28" s="9" t="s">
+      <c r="R28" s="10"/>
+      <c r="S28" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S28" s="10"/>
-      <c r="T28" s="12">
+      <c r="T28" s="10"/>
+      <c r="U28" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="39" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>63</v>
       </c>
@@ -2535,24 +2613,25 @@
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
-      <c r="O29" s="9" t="s">
+      <c r="O29" s="10"/>
+      <c r="P29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P29" s="9" t="s">
+      <c r="Q29" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Q29" s="9" t="s">
+      <c r="R29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="R29" s="10"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="12">
+      <c r="T29" s="10"/>
+      <c r="U29" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="C30" s="7"/>
       <c r="D30" s="3"/>
@@ -2568,12 +2647,13 @@
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
       <c r="P30" s="10"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="9"/>
       <c r="S30" s="10"/>
-      <c r="T30" s="12"/>
-    </row>
-    <row r="31" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T30" s="10"/>
+      <c r="U30" s="12"/>
+    </row>
+    <row r="31" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
         <f>COUNTA(A7:A29)/COUNTA(B7:B29)</f>
         <v>0.52173913043478259</v>
@@ -2582,7 +2662,7 @@
         <v>66</v>
       </c>
       <c r="E31" s="16">
-        <f t="shared" ref="E31:N31" si="0">COUNTA(E7:E30)</f>
+        <f t="shared" ref="E31:O31" si="0">COUNTA(E7:E30)</f>
         <v>1</v>
       </c>
       <c r="F31" s="16">
@@ -2615,19 +2695,19 @@
       </c>
       <c r="M31" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N31" s="16">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O31" s="16">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O31" s="16">
-        <f t="shared" ref="O31" si="1">COUNTA(O7:O30)</f>
+      <c r="P31" s="16">
+        <f t="shared" ref="P31" si="1">COUNTA(P7:P30)</f>
         <v>4</v>
-      </c>
-      <c r="P31" s="16">
-        <f>COUNTA(P7:P30)</f>
-        <v>3</v>
       </c>
       <c r="Q31" s="16">
         <f>COUNTA(Q7:Q30)</f>
@@ -2635,27 +2715,31 @@
       </c>
       <c r="R31" s="16">
         <f>COUNTA(R7:R30)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S31" s="16">
         <f>COUNTA(S7:S30)</f>
+        <v>2</v>
+      </c>
+      <c r="T31" s="16">
+        <f>COUNTA(T7:T30)</f>
         <v>1</v>
       </c>
-      <c r="T31" s="18">
+      <c r="U31" s="18">
         <f>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</f>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A5:R5"/>
+    <mergeCell ref="A5:S5"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E31:S31">
+  <conditionalFormatting sqref="E31:T31">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2665,7 +2749,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T7:T30">
+  <conditionalFormatting sqref="U7:U30">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Added keywords for fgDeGender
</commit_message>
<xml_diff>
--- a/JSON/fgDeGender_Trefwoorden.xlsx
+++ b/JSON/fgDeGender_Trefwoorden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6F36B5-198D-9747-AA0B-EDCE5C4B087C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196B5A89-70C6-C543-8C6E-E86AFB0A2FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26440" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
   </bookViews>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
   <si>
     <t>Albert</t>
-  </si>
-  <si>
-    <t>de Koning</t>
   </si>
   <si>
     <t>Experimenteel</t>
@@ -256,12 +253,21 @@
   </si>
   <si>
     <t>Museum</t>
+  </si>
+  <si>
+    <t>Koning</t>
+  </si>
+  <si>
+    <t>Zelfexpressie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -379,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -439,6 +445,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -448,17 +464,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="47">
     <dxf>
       <font>
         <b val="0"/>
@@ -476,6 +489,24 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1000,6 +1031,24 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1285,64 +1334,65 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:U31" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43" totalsRowDxfId="42">
-  <autoFilter ref="A6:U30" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
-  <tableColumns count="21">
-    <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="20">
-      <totalsRowFormula>COUNTA(A7:A29)/COUNTA(B7:B29)</totalsRowFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:V31" totalsRowCount="1" headerRowDxfId="46" dataDxfId="45" totalsRowDxfId="44">
+  <autoFilter ref="A6:V30" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
+  <tableColumns count="22">
+    <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="21">
+      <totalsRowFormula>COUNTIF(A7:A29,"✓")/COUNTA(B7:B29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="40" totalsRowDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="39" totalsRowDxfId="18"/>
-    <tableColumn id="18" xr3:uid="{F762D242-8B7F-1147-BBFB-3246F5000811}" name="eventueel voorstel voor _x000a_nieuw trefwoord" totalsRowLabel="#" dataDxfId="38" totalsRowDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{3B6A13EE-99F5-7441-8057-E1A06F70075A}" name="Abstract" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="16">
+    <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="42" totalsRowDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="41" totalsRowDxfId="19"/>
+    <tableColumn id="18" xr3:uid="{F762D242-8B7F-1147-BBFB-3246F5000811}" name="eventueel voorstel voor _x000a_nieuw trefwoord" totalsRowLabel="#" dataDxfId="40" totalsRowDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{3B6A13EE-99F5-7441-8057-E1A06F70075A}" name="Abstract" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="17">
       <totalsRowFormula>COUNTA(E7:E30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E9B92604-5273-624A-92B0-22FFB11BEC40}" name="Architectuur" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="15">
+    <tableColumn id="4" xr3:uid="{E9B92604-5273-624A-92B0-22FFB11BEC40}" name="Architectuur" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="16">
       <totalsRowFormula>COUNTA(F7:F30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{832AF978-DCE3-DA47-B36A-9D928FCF0BF1}" name="Conceptueel" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="14">
+    <tableColumn id="6" xr3:uid="{832AF978-DCE3-DA47-B36A-9D928FCF0BF1}" name="Conceptueel" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="15">
       <totalsRowFormula>COUNTA(G7:G30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64143930-3345-DA4D-9135-20E16BCCB08E}" name="Concert" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="13">
+    <tableColumn id="7" xr3:uid="{64143930-3345-DA4D-9135-20E16BCCB08E}" name="Concert" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="14">
       <totalsRowFormula>COUNTA(H7:H30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="12">
+    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="13">
       <totalsRowFormula>COUNTA(I7:I30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="11">
+    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="12">
       <totalsRowFormula>COUNTA(J7:J30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="10">
+    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="11">
       <totalsRowFormula>COUNTA(K7:K30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="9">
+    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="10">
       <totalsRowFormula>COUNTA(L7:L30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{34A8085A-25B7-B64C-9185-7DCD6F2A68CF}" name="Museum" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="8">
+    <tableColumn id="5" xr3:uid="{34A8085A-25B7-B64C-9185-7DCD6F2A68CF}" name="Museum" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="9">
       <totalsRowFormula>COUNTA(M7:M30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="7">
+    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="8">
       <totalsRowFormula>COUNTA(N7:N30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="6">
+    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="7">
       <totalsRowFormula>COUNTA(O7:O30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="5">
+    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="6">
       <totalsRowFormula>COUNTA(P7:P30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="4">
+    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="5">
       <totalsRowFormula>COUNTA(Q7:Q30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="3">
+    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="4">
       <totalsRowFormula>COUNTA(R7:R30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="2">
+    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="3">
       <totalsRowFormula>COUNTA(S7:S30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="1">
-      <totalsRowFormula>COUNTA(T7:T30)</totalsRowFormula>
+    <tableColumn id="20" xr3:uid="{0BCDD0DC-39BA-EE43-BE8C-DB82549B10E5}" name="Zelfexpressie" dataDxfId="22" totalsRowDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="1">
+      <totalsRowFormula>COUNTA(U7:U30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="0">
+    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="0">
       <calculatedColumnFormula>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</totalsRowFormula>
@@ -1669,10 +1719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB03C53-D149-8D47-9F9C-2A5FA6F563CA}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -1687,148 +1737,152 @@
     <col min="11" max="11" width="10.83203125" style="1"/>
     <col min="12" max="15" width="10.83203125" style="1" customWidth="1"/>
     <col min="16" max="18" width="10.83203125" style="1"/>
-    <col min="19" max="19" width="13.83203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.83203125" style="1"/>
-    <col min="21" max="21" width="11.5" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="1"/>
+    <col min="19" max="20" width="13.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" style="1"/>
+    <col min="22" max="22" width="11.5" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="V1" s="19">
+        <v>45774</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="28"/>
+      <c r="B2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="U1" s="19">
-        <v>45774</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-    </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="25"/>
+    </row>
+    <row r="6" spans="1:25" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="V6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="10"/>
@@ -1839,35 +1893,36 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
-      <c r="M7" s="27" t="s">
-        <v>72</v>
+      <c r="M7" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="26" t="s">
+      <c r="Q7" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="R7" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
-      <c r="U7" s="12">
+      <c r="U7" s="10"/>
+      <c r="V7" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>19</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="10"/>
@@ -1886,19 +1941,22 @@
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
-      <c r="U8" s="12">
+      <c r="U8" s="10"/>
+      <c r="V8" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="38" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:25" ht="52" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="B9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="10"/>
@@ -1906,8 +1964,12 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="J9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
@@ -1916,31 +1978,32 @@
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
       <c r="S9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="T9" s="10"/>
-      <c r="U9" s="12">
+        <v>11</v>
+      </c>
+      <c r="T9" s="9"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="55" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="55" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -1950,27 +2013,28 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
-      <c r="U10" s="12">
+      <c r="U10" s="10"/>
+      <c r="V10" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="65" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="65" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>24</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="10"/>
@@ -1978,14 +2042,14 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -1993,21 +2057,22 @@
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
-      <c r="U11" s="12">
+      <c r="U11" s="10"/>
+      <c r="V11" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="39" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>26</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="10"/>
@@ -2017,37 +2082,38 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
-      <c r="U12" s="12">
+      <c r="U12" s="10"/>
+      <c r="V12" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -2065,32 +2131,33 @@
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
-      <c r="U13" s="12">
+      <c r="U13" s="10"/>
+      <c r="V13" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="58" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="58" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="10"/>
       <c r="F14" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -2101,22 +2168,26 @@
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="U14" s="12">
+      <c r="T14" s="10"/>
+      <c r="U14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="V14" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="Y14" s="26"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="B15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>34</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="10"/>
@@ -2135,19 +2206,20 @@
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
-      <c r="U15" s="12">
+      <c r="U15" s="10"/>
+      <c r="V15" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="47" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="10"/>
@@ -2158,7 +2230,7 @@
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" s="9"/>
       <c r="N16" s="10"/>
@@ -2168,21 +2240,22 @@
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
-      <c r="U16" s="12">
+      <c r="U16" s="10"/>
+      <c r="V16" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="65" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="65" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="10"/>
@@ -2190,38 +2263,39 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
-      <c r="U17" s="12">
+      <c r="U17" s="10"/>
+      <c r="V17" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="10"/>
@@ -2240,19 +2314,22 @@
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
-      <c r="U18" s="12">
+      <c r="U18" s="10"/>
+      <c r="V18" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:22" ht="62" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="B19" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="10"/>
@@ -2270,22 +2347,25 @@
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="12">
+      <c r="T19" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="U19" s="10"/>
+      <c r="V19" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="52" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="52" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="10"/>
@@ -2294,11 +2374,11 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="10"/>
@@ -2306,23 +2386,24 @@
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
-      <c r="U20" s="12">
+      <c r="U20" s="10"/>
+      <c r="V20" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="65" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="65" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>47</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="10"/>
@@ -2330,7 +2411,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -2343,19 +2424,20 @@
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
-      <c r="U21" s="12">
+      <c r="U21" s="10"/>
+      <c r="V21" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="52" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="52" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="10"/>
@@ -2364,7 +2446,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -2376,33 +2458,34 @@
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
-      <c r="U22" s="12">
+      <c r="U22" s="10"/>
+      <c r="V22" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="65" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" ht="65" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -2415,38 +2498,39 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
-      <c r="U23" s="12">
+      <c r="U23" s="10"/>
+      <c r="V23" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="60" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="60" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>53</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
@@ -2454,19 +2538,20 @@
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
-      <c r="U24" s="12">
+      <c r="U24" s="10"/>
+      <c r="V24" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="10"/>
@@ -2485,19 +2570,20 @@
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
-      <c r="U25" s="12">
+      <c r="U25" s="10"/>
+      <c r="V25" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
       <c r="B26" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="10"/>
@@ -2514,25 +2600,26 @@
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S26" s="10"/>
       <c r="T26" s="10"/>
-      <c r="U26" s="12">
+      <c r="U26" s="10"/>
+      <c r="V26" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="39" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="10"/>
@@ -2547,33 +2634,40 @@
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
       <c r="T27" s="10"/>
-      <c r="U27" s="12">
+      <c r="U27" s="10"/>
+      <c r="V27" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="38" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
+    <row r="28" spans="1:22" ht="58" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="B28" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
+      <c r="F28" s="22" t="s">
+        <v>10</v>
+      </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="J28" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
@@ -2583,24 +2677,25 @@
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
       <c r="S28" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="T28" s="10"/>
-      <c r="U28" s="12">
+        <v>11</v>
+      </c>
+      <c r="T28" s="9"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="39" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="39" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="10"/>
@@ -2615,23 +2710,24 @@
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="R29" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="R29" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
-      <c r="U29" s="12">
+      <c r="U29" s="10"/>
+      <c r="V29" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="C30" s="7"/>
       <c r="D30" s="3"/>
@@ -2651,15 +2747,16 @@
       <c r="R30" s="9"/>
       <c r="S30" s="10"/>
       <c r="T30" s="10"/>
-      <c r="U30" s="12"/>
-    </row>
-    <row r="31" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U30" s="10"/>
+      <c r="V30" s="12"/>
+    </row>
+    <row r="31" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
-        <f>COUNTA(A7:A29)/COUNTA(B7:B29)</f>
-        <v>0.52173913043478259</v>
+        <f>COUNTIF(A7:A29,"✓")/COUNTA(B7:B29)</f>
+        <v>0.56521739130434778</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E31" s="16">
         <f t="shared" ref="E31:O31" si="0">COUNTA(E7:E30)</f>
@@ -2667,7 +2764,7 @@
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" s="16">
         <f t="shared" si="0"/>
@@ -2683,11 +2780,11 @@
       </c>
       <c r="J31" s="16">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K31" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L31" s="16">
         <f t="shared" si="0"/>
@@ -2721,13 +2818,14 @@
         <f>COUNTA(S7:S30)</f>
         <v>2</v>
       </c>
-      <c r="T31" s="16">
-        <f>COUNTA(T7:T30)</f>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16">
+        <f>COUNTA(U7:U30)</f>
         <v>1</v>
       </c>
-      <c r="U31" s="18">
+      <c r="V31" s="18">
         <f>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</f>
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2739,7 +2837,7 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E31:T31">
+  <conditionalFormatting sqref="E31:U31">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2749,7 +2847,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U7:U30">
+  <conditionalFormatting sqref="V7:V30">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Keywords for fgDeGender member
</commit_message>
<xml_diff>
--- a/JSON/fgDeGender_Trefwoorden.xlsx
+++ b/JSON/fgDeGender_Trefwoorden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7A8505-04B9-0A49-8FC4-856ACFA0BC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB15DD7-8055-6246-941D-AA67B6A2FD6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26440" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="74">
   <si>
     <t>Albert</t>
   </si>
@@ -459,6 +459,9 @@
       <alignment horizontal="left" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -466,9 +469,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1725,7 +1725,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -1747,66 +1747,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="V1" s="19">
         <v>45774</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
       <c r="T5" s="25"/>
     </row>
     <row r="6" spans="1:25" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -1905,7 +1905,7 @@
       <c r="Q7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="R7" s="23" t="s">
         <v>8</v>
       </c>
       <c r="S7" s="10"/>
@@ -1917,7 +1917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="60" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>62</v>
       </c>
@@ -1929,7 +1929,9 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="22" t="s">
+        <v>10</v>
+      </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -1937,18 +1939,22 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
+      <c r="N8" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
+      <c r="R8" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
       <c r="V8" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="52" x14ac:dyDescent="0.3">
@@ -2589,7 +2595,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="30" x14ac:dyDescent="0.3">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="28" t="s">
         <v>70</v>
       </c>
       <c r="B26" s="13" t="s">
@@ -2777,7 +2783,7 @@
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31" s="16">
         <f t="shared" si="0"/>
@@ -2809,7 +2815,7 @@
       </c>
       <c r="N31" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O31" s="16">
         <f t="shared" si="0"/>
@@ -2825,7 +2831,7 @@
       </c>
       <c r="R31" s="16">
         <f>COUNTA(R7:R30)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S31" s="16">
         <f>COUNTA(S7:S30)</f>
@@ -2838,7 +2844,7 @@
       </c>
       <c r="V31" s="18">
         <f>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</f>
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New keyword for Multiple-Exposure
</commit_message>
<xml_diff>
--- a/JSON/fgDeGender_Trefwoorden.xlsx
+++ b/JSON/fgDeGender_Trefwoorden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B7DF46-2C51-D748-8AC3-EE9CC5D548B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C91DCA-C2AD-6F45-A40C-CADCE7980EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26440" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="75">
   <si>
     <t>Albert</t>
   </si>
@@ -128,9 +128,6 @@
     <t>achternaam</t>
   </si>
   <si>
-    <t>documentaire?</t>
-  </si>
-  <si>
     <t>Krüsemann</t>
   </si>
   <si>
@@ -230,13 +227,6 @@
     <t>Gezien?</t>
   </si>
   <si>
-    <t>eventueel voorstel voor 
-nieuw trefwoord</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Spelregels</t>
   </si>
   <si>
@@ -262,6 +252,15 @@
   </si>
   <si>
     <t>Mixed-Media</t>
+  </si>
+  <si>
+    <t>Meervoudige-Belichting</t>
+  </si>
+  <si>
+    <t>Drone</t>
+  </si>
+  <si>
+    <t>#/persoon</t>
   </si>
 </sst>
 </file>
@@ -388,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -441,6 +440,18 @@
     </xf>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -449,29 +460,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="51">
     <dxf>
       <font>
         <b val="0"/>
@@ -828,7 +821,24 @@
         <sz val="16"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1120,7 +1130,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1192,7 +1202,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1241,13 +1251,48 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="16"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1284,14 +1329,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1299,6 +1342,23 @@
         <sz val="16"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
@@ -1322,39 +1382,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1370,68 +1397,76 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:W31" totalsRowCount="1" headerRowDxfId="46" dataDxfId="48" totalsRowDxfId="47">
-  <autoFilter ref="A6:W30" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
-  <tableColumns count="23">
-    <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:X31" totalsRowCount="1" headerRowDxfId="50" dataDxfId="49" totalsRowDxfId="48">
+  <autoFilter ref="A6:X30" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
+  <tableColumns count="24">
+    <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="23">
       <totalsRowFormula>COUNTIF(A7:A29,"✓")/COUNTA(B7:B29)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="44" totalsRowDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="43" totalsRowDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{F762D242-8B7F-1147-BBFB-3246F5000811}" name="eventueel voorstel voor _x000a_nieuw trefwoord" totalsRowLabel="#" dataDxfId="42" totalsRowDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{3B6A13EE-99F5-7441-8057-E1A06F70075A}" name="Abstract" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="18">
+    <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="46" totalsRowDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="45" totalsRowDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{3B6A13EE-99F5-7441-8057-E1A06F70075A}" name="Abstract" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="20">
+      <totalsRowFormula>COUNTA(D7:D30)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{E9B92604-5273-624A-92B0-22FFB11BEC40}" name="Architectuur" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="19">
       <totalsRowFormula>COUNTA(E7:E30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E9B92604-5273-624A-92B0-22FFB11BEC40}" name="Architectuur" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="17">
+    <tableColumn id="6" xr3:uid="{832AF978-DCE3-DA47-B36A-9D928FCF0BF1}" name="Conceptueel" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="18">
       <totalsRowFormula>COUNTA(F7:F30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{832AF978-DCE3-DA47-B36A-9D928FCF0BF1}" name="Conceptueel" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="16">
+    <tableColumn id="7" xr3:uid="{64143930-3345-DA4D-9135-20E16BCCB08E}" name="Concert" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="17">
       <totalsRowFormula>COUNTA(G7:G30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64143930-3345-DA4D-9135-20E16BCCB08E}" name="Concert" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="15">
+    <tableColumn id="26" xr3:uid="{32897D46-8F9F-3E49-B198-8C097B1CCB00}" name="Drone" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="16">
       <totalsRowFormula>COUNTA(H7:H30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="14">
+    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="15">
       <totalsRowFormula>COUNTA(I7:I30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="13">
+    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="14">
       <totalsRowFormula>COUNTA(J7:J30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="12">
+    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="13">
       <totalsRowFormula>COUNTA(K7:K30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="11">
+    <tableColumn id="25" xr3:uid="{2E8FBDE5-5DE6-8F45-9CD3-D96DE8979E6D}" name="Meervoudige-Belichting" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="12">
       <totalsRowFormula>COUNTA(L7:L30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{34A8085A-25B7-B64C-9185-7DCD6F2A68CF}" name="Museum" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="10">
+    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="11">
       <totalsRowFormula>COUNTA(M7:M30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{5B57471E-1B52-2048-A846-292B312EF0C6}" name="Mixed-Media" dataDxfId="32" totalsRowDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="8">
+    <tableColumn id="5" xr3:uid="{34A8085A-25B7-B64C-9185-7DCD6F2A68CF}" name="Museum" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="10">
+      <totalsRowFormula>COUNTA(N7:N30)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="23" xr3:uid="{5B57471E-1B52-2048-A846-292B312EF0C6}" name="Mixed-Media" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="9">
       <totalsRowFormula>COUNTA(O7:O30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="7">
+    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="8">
       <totalsRowFormula>COUNTA(P7:P30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="6">
+    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="7">
       <totalsRowFormula>COUNTA(Q7:Q30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="5">
+    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="6">
       <totalsRowFormula>COUNTA(R7:R30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="4">
+    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="5">
       <totalsRowFormula>COUNTA(S7:S30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="3">
+    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="4">
       <totalsRowFormula>COUNTA(T7:T30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{0BCDD0DC-39BA-EE43-BE8C-DB82549B10E5}" name="Zelfexpressie" dataDxfId="25" totalsRowDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="1">
+    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="3">
+      <totalsRowFormula>COUNTA(U7:U30)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="20" xr3:uid="{0BCDD0DC-39BA-EE43-BE8C-DB82549B10E5}" name="Zelfexpressie" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="2">
       <totalsRowFormula>COUNTA(V7:V30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="0">
-      <calculatedColumnFormula>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</calculatedColumnFormula>
+    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="1">
+      <totalsRowFormula>COUNTA(W7:W30)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#/persoon" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="0">
+      <calculatedColumnFormula>COUNTA(#REF!)</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1756,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB03C53-D149-8D47-9F9C-2A5FA6F563CA}">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -1767,165 +1802,164 @@
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="10" width="10.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="16" width="10.83203125" style="1" customWidth="1"/>
-    <col min="17" max="19" width="10.83203125" style="1"/>
-    <col min="20" max="21" width="13.83203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" style="1"/>
-    <col min="23" max="23" width="11.5" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="10" width="10.83203125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="17" width="10.83203125" style="1" customWidth="1"/>
+    <col min="18" max="20" width="10.83203125" style="1"/>
+    <col min="21" max="22" width="13.83203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" style="1"/>
+    <col min="24" max="24" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="X1" s="14">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="W1" s="14">
-        <v>45774</v>
-      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23" t="s">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
+      <c r="B4" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="19"/>
+    </row>
+    <row r="6" spans="1:27" s="2" customFormat="1" ht="127" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="O6" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="T6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="V6" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="W6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="X6" s="24" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="19"/>
-    </row>
-    <row r="6" spans="1:26" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="M6" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="N6" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="O6" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="R6" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="S6" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="T6" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="U6" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="V6" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="W6" s="29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="45" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1934,31 +1968,31 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="18"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
-      <c r="R7" s="17" t="s">
+      <c r="R7" s="6"/>
+      <c r="S7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="17" t="s">
+      <c r="T7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="T7" s="6"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
-      <c r="W7" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W7" s="6"/>
+      <c r="X7" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" ht="60" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>17</v>
@@ -1966,11 +2000,11 @@
       <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="16" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="16" t="s">
         <v>10</v>
       </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1979,27 +2013,27 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="6"/>
+      <c r="P8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="6"/>
+      <c r="T8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="T8" s="6"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
-      <c r="W8" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W8" s="6"/>
+      <c r="X8" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="52" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" ht="52" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>19</v>
@@ -2007,7 +2041,7 @@
       <c r="C9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -2019,7 +2053,7 @@
       <c r="K9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="5"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -2027,34 +2061,34 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
-      <c r="T9" s="5" t="s">
+      <c r="T9" s="6"/>
+      <c r="U9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="U9" s="5"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="V9" s="5"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" ht="43" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="16" t="s">
+      <c r="G10" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="H10" s="16"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -2063,25 +2097,25 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="5" t="s">
+      <c r="Q10" s="6"/>
+      <c r="R10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="S10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S10" s="6"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
-      <c r="W10" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W10" s="6"/>
+      <c r="X10" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="65" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" ht="65" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>22</v>
@@ -2089,7 +2123,7 @@
       <c r="C11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -2101,28 +2135,28 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-      <c r="N11" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="O11" s="5" t="s">
+      <c r="N11" s="6"/>
+      <c r="O11" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="5"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
-      <c r="W11" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W11" s="6"/>
+      <c r="X11" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" ht="39" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>24</v>
@@ -2130,7 +2164,7 @@
       <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -2140,30 +2174,30 @@
       <c r="K12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="5"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="5" t="s">
+      <c r="Q12" s="6"/>
+      <c r="R12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="S12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W12" s="6"/>
+      <c r="X12" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>26</v>
@@ -2171,9 +2205,7 @@
       <c r="C13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -2192,27 +2224,27 @@
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
-      <c r="W13" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>1</v>
+      <c r="W13" s="6"/>
+      <c r="X13" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="58" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" ht="58" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="16" t="s">
         <v>10</v>
       </c>
+      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -2230,30 +2262,30 @@
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
-      <c r="V14" s="5" t="s">
+      <c r="V14" s="6"/>
+      <c r="W14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="W14" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="X14" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
-      <c r="Z14" s="20"/>
+      <c r="AA14" s="20"/>
     </row>
-    <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>9</v>
       </c>
+      <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -2265,33 +2297,33 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="5" t="s">
+      <c r="Q15" s="6"/>
+      <c r="R15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R15" s="5" t="s">
+      <c r="S15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S15" s="6"/>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
-      <c r="W15" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W15" s="6"/>
+      <c r="X15" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" ht="47" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -2299,12 +2331,12 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="6"/>
+      <c r="M16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M16" s="5"/>
       <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
+      <c r="O16" s="5"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
@@ -2312,23 +2344,23 @@
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
-      <c r="W16" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W16" s="6"/>
+      <c r="X16" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="65" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="65" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -2340,40 +2372,40 @@
       <c r="K17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="6"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
-      <c r="P17" s="5" t="s">
+      <c r="P17" s="6"/>
+      <c r="Q17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
-      <c r="W17" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W17" s="6"/>
+      <c r="X17" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="65" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="65" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="16" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="16" t="s">
         <v>10</v>
       </c>
+      <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="5" t="s">
@@ -2394,23 +2426,23 @@
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
-      <c r="W18" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W18" s="6"/>
+      <c r="X18" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="62" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="62" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -2427,29 +2459,29 @@
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
-      <c r="U19" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="V19" s="6"/>
-      <c r="W19" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="U19" s="6"/>
+      <c r="V19" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W19" s="6"/>
+      <c r="X19" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="52" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="52" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -2457,38 +2489,38 @@
         <v>15</v>
       </c>
       <c r="K20" s="6"/>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="6"/>
+      <c r="M20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M20" s="5"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="6"/>
+      <c r="O20" s="5"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
-      <c r="S20" s="5" t="s">
+      <c r="S20" s="6"/>
+      <c r="T20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="T20" s="6"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
-      <c r="W20" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W20" s="6"/>
+      <c r="X20" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="65" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="97" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -2498,34 +2530,40 @@
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="L21" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
+      <c r="R21" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
-      <c r="W21" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>1</v>
+      <c r="W21" s="6"/>
+      <c r="X21" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
+        <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="52" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" ht="52" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -2534,8 +2572,10 @@
       <c r="J22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+      <c r="K22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L22" s="5"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -2546,30 +2586,30 @@
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
-      <c r="W22" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>1</v>
+      <c r="W22" s="6"/>
+      <c r="X22" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
+        <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="65" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="65" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="16" t="s">
+      <c r="D23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="5" t="s">
+      <c r="E23" s="6"/>
+      <c r="F23" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="5" t="s">
         <v>1</v>
@@ -2579,36 +2619,36 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="5"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
-      <c r="W23" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W23" s="6"/>
+      <c r="X23" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="60" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" ht="60" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="5" t="s">
@@ -2618,37 +2658,37 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
-      <c r="O24" s="5" t="s">
+      <c r="O24" s="6"/>
+      <c r="P24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
-      <c r="W24" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W24" s="6"/>
+      <c r="X24" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="58" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" ht="58" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="16" t="s">
+      <c r="D25" s="6"/>
+      <c r="E25" s="16" t="s">
         <v>10</v>
       </c>
+      <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -2659,41 +2699,41 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
-      <c r="Q25" s="5" t="s">
+      <c r="Q25" s="6"/>
+      <c r="R25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R25" s="6"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
-      <c r="V25" s="5" t="s">
+      <c r="V25" s="6"/>
+      <c r="W25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="W25" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="X25" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="45" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="16" t="s">
+      <c r="D26" s="16" t="s">
         <v>9</v>
       </c>
+      <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="16" t="s">
+      <c r="G26" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="H26" s="16"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -2704,29 +2744,29 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="S26" s="5" t="s">
+      <c r="S26" s="6"/>
+      <c r="T26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="T26" s="6"/>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
-      <c r="W26" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W26" s="6"/>
+      <c r="X26" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="39" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -2739,35 +2779,35 @@
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
-      <c r="Q27" s="5" t="s">
+      <c r="Q27" s="6"/>
+      <c r="R27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R27" s="6"/>
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
-      <c r="W27" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W27" s="6"/>
+      <c r="X27" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="58" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="58" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="16" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="16" t="s">
         <v>10</v>
       </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -2783,28 +2823,28 @@
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
       <c r="S28" s="6"/>
-      <c r="T28" s="5" t="s">
+      <c r="T28" s="6"/>
+      <c r="U28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="U28" s="5"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="V28" s="5"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="39" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2817,28 +2857,28 @@
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
-      <c r="Q29" s="5" t="s">
+      <c r="Q29" s="6"/>
+      <c r="R29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R29" s="5" t="s">
+      <c r="S29" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S29" s="5" t="s">
+      <c r="T29" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="T29" s="6"/>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
-      <c r="W29" s="7">
-        <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
-nieuw trefwoord]:[Zwart-wit]])</f>
+      <c r="W29" s="6"/>
+      <c r="X29" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="3"/>
+      <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -2853,27 +2893,29 @@
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="5"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
-      <c r="W30" s="7"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="7"/>
     </row>
-    <row r="31" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <f>COUNTIF(A7:A29,"✓")/COUNTA(B7:B29)</f>
-        <v>0.82608695652173914</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>65</v>
+        <v>0.91304347826086951</v>
+      </c>
+      <c r="D31" s="11">
+        <f t="shared" ref="D31:Q31" si="0">COUNTA(D7:D30)</f>
+        <v>4</v>
       </c>
       <c r="E31" s="11">
-        <f t="shared" ref="E31:P31" si="0">COUNTA(E7:E30)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="F31" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G31" s="11">
         <f t="shared" si="0"/>
@@ -2881,7 +2923,7 @@
       </c>
       <c r="H31" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I31" s="11">
         <f t="shared" si="0"/>
@@ -2893,32 +2935,35 @@
       </c>
       <c r="K31" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L31" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M31" s="11">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N31" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N31" s="11"/>
       <c r="O31" s="11">
+        <f>COUNTA(O7:O30)</f>
+        <v>1</v>
+      </c>
+      <c r="P31" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P31" s="11">
+      <c r="Q31" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q31" s="11">
-        <f t="shared" ref="Q31" si="1">COUNTA(Q7:Q30)</f>
-        <v>6</v>
-      </c>
       <c r="R31" s="11">
-        <f>COUNTA(R7:R30)</f>
-        <v>5</v>
+        <f t="shared" ref="R31" si="1">COUNTA(R7:R30)</f>
+        <v>7</v>
       </c>
       <c r="S31" s="11">
         <f>COUNTA(S7:S30)</f>
@@ -2926,29 +2971,36 @@
       </c>
       <c r="T31" s="11">
         <f>COUNTA(T7:T30)</f>
+        <v>5</v>
+      </c>
+      <c r="U31" s="11">
+        <f>COUNTA(U7:U30)</f>
         <v>2</v>
       </c>
-      <c r="U31" s="11"/>
       <c r="V31" s="11">
         <f>COUNTA(V7:V30)</f>
+        <v>1</v>
+      </c>
+      <c r="W31" s="11">
+        <f>COUNTA(W7:W30)</f>
         <v>2</v>
       </c>
-      <c r="W31" s="13">
+      <c r="X31" s="13">
         <f>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</f>
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A5:T5"/>
+    <mergeCell ref="A5:U5"/>
     <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E31:V31">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="X7:X30">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2956,17 +3008,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W7:W30">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2977,6 +3019,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D31:W31">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Moved all level3URLs for fgDeGender to their site.
</commit_message>
<xml_diff>
--- a/JSON/fgDeGender_Trefwoorden.xlsx
+++ b/JSON/fgDeGender_Trefwoorden.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D676FB-0F23-5D4A-82E8-3652A04C15C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD475C1E-EC5C-BF4E-B9AF-A403B711D102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26440" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="26220" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="76">
   <si>
     <t>Albert</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Landschap</t>
   </si>
   <si>
-    <t xml:space="preserve">    ‣ Maximaal 3 trefwoorden per persoon</t>
-  </si>
-  <si>
     <t>Anke</t>
   </si>
   <si>
@@ -261,6 +258,12 @@
   </si>
   <si>
     <t>Documentary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ‣ Maximaal 2 trefwoorden per persoon</t>
+  </si>
+  <si>
+    <t>Vervloed</t>
   </si>
 </sst>
 </file>
@@ -387,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -460,6 +463,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,24 +934,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="16"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
@@ -1221,6 +1212,24 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1433,76 +1442,76 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:Y31" totalsRowCount="1" headerRowDxfId="52" dataDxfId="51" totalsRowDxfId="50">
-  <autoFilter ref="A6:Y30" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:Y32" totalsRowCount="1" headerRowDxfId="52" dataDxfId="51" totalsRowDxfId="50">
+  <autoFilter ref="A6:Y31" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
   <tableColumns count="25">
     <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="24">
-      <totalsRowFormula>COUNTIF(A7:A29,"✓")/COUNTA(B7:B29)</totalsRowFormula>
+      <totalsRowFormula>COUNTIF(A7:A30,"✓")/COUNTA(B7:B30)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="48" totalsRowDxfId="23"/>
     <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="47" totalsRowDxfId="22"/>
     <tableColumn id="3" xr3:uid="{3B6A13EE-99F5-7441-8057-E1A06F70075A}" name="Abstract" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="21">
-      <totalsRowFormula>COUNTA(D7:D30)</totalsRowFormula>
+      <totalsRowFormula>COUNTA(D7:D31)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{E9B92604-5273-624A-92B0-22FFB11BEC40}" name="Architectuur" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="20">
-      <totalsRowFormula>COUNTA(E7:E30)</totalsRowFormula>
+      <totalsRowFormula>COUNTA(E7:E31)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{832AF978-DCE3-DA47-B36A-9D928FCF0BF1}" name="Conceptueel" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="19">
-      <totalsRowFormula>COUNTA(F7:F30)</totalsRowFormula>
+      <totalsRowFormula>COUNTA(F7:F31)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{64143930-3345-DA4D-9135-20E16BCCB08E}" name="Concert" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="18">
-      <totalsRowFormula>COUNTA(G7:G30)</totalsRowFormula>
+      <totalsRowFormula>COUNTA(G7:G31)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="26" xr3:uid="{32897D46-8F9F-3E49-B198-8C097B1CCB00}" name="Drone" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="17">
-      <totalsRowFormula>COUNTA(H7:H30)</totalsRowFormula>
+      <totalsRowFormula>COUNTA(H7:H31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{E9A6A14D-691C-F049-BD47-F88709944822}" name="Documentary" dataDxfId="25" totalsRowDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="15">
-      <totalsRowFormula>COUNTA(J7:J30)</totalsRowFormula>
+    <tableColumn id="18" xr3:uid="{E9A6A14D-691C-F049-BD47-F88709944822}" name="Documentary" dataDxfId="41" totalsRowDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="15">
+      <totalsRowFormula>COUNTA(J7:J31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="14">
-      <totalsRowFormula>COUNTA(K7:K30)</totalsRowFormula>
+    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="14">
+      <totalsRowFormula>COUNTA(K7:K31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="13">
-      <totalsRowFormula>COUNTA(L7:L30)</totalsRowFormula>
+    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="13">
+      <totalsRowFormula>COUNTA(L7:L31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{2E8FBDE5-5DE6-8F45-9CD3-D96DE8979E6D}" name="Meervoudige-Belichting" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="12">
-      <totalsRowFormula>COUNTA(M7:M30)</totalsRowFormula>
+    <tableColumn id="25" xr3:uid="{2E8FBDE5-5DE6-8F45-9CD3-D96DE8979E6D}" name="Meervoudige-Belichting" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="12">
+      <totalsRowFormula>COUNTA(M7:M31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="11">
-      <totalsRowFormula>COUNTA(N7:N30)</totalsRowFormula>
+    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="11">
+      <totalsRowFormula>COUNTA(N7:N31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{34A8085A-25B7-B64C-9185-7DCD6F2A68CF}" name="Museum" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="10">
-      <totalsRowFormula>COUNTA(O7:O30)</totalsRowFormula>
+    <tableColumn id="5" xr3:uid="{34A8085A-25B7-B64C-9185-7DCD6F2A68CF}" name="Museum" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="10">
+      <totalsRowFormula>COUNTA(O7:O31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{5B57471E-1B52-2048-A846-292B312EF0C6}" name="Mixed-Media" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="9">
-      <totalsRowFormula>COUNTA(P7:P30)</totalsRowFormula>
+    <tableColumn id="23" xr3:uid="{5B57471E-1B52-2048-A846-292B312EF0C6}" name="Mixed-Media" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="9">
+      <totalsRowFormula>COUNTA(P7:P31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="8">
-      <totalsRowFormula>COUNTA(Q7:Q30)</totalsRowFormula>
+    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="8">
+      <totalsRowFormula>COUNTA(Q7:Q31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="7">
-      <totalsRowFormula>COUNTA(R7:R30)</totalsRowFormula>
+    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="7">
+      <totalsRowFormula>COUNTA(R7:R31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="6">
-      <totalsRowFormula>COUNTA(S7:S30)</totalsRowFormula>
+    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="6">
+      <totalsRowFormula>COUNTA(S7:S31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="5">
-      <totalsRowFormula>COUNTA(T7:T30)</totalsRowFormula>
+    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="5">
+      <totalsRowFormula>COUNTA(T7:T31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="4">
-      <totalsRowFormula>COUNTA(U7:U30)</totalsRowFormula>
+    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="4">
+      <totalsRowFormula>COUNTA(U7:U31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="3">
-      <totalsRowFormula>COUNTA(V7:V30)</totalsRowFormula>
+    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="3">
+      <totalsRowFormula>COUNTA(V7:V31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{0BCDD0DC-39BA-EE43-BE8C-DB82549B10E5}" name="Zelfexpressie" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="2">
-      <totalsRowFormula>COUNTA(W7:W30)</totalsRowFormula>
+    <tableColumn id="20" xr3:uid="{0BCDD0DC-39BA-EE43-BE8C-DB82549B10E5}" name="Zelfexpressie" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="2">
+      <totalsRowFormula>COUNTA(W7:W31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="1">
-      <totalsRowFormula>COUNTA(X7:X30)</totalsRowFormula>
+    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="1">
+      <totalsRowFormula>COUNTA(X7:X31)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#/persoon" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="0">
+    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#/persoon" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="0">
       <calculatedColumnFormula>COUNTA(#REF!)</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</totalsRowFormula>
     </tableColumn>
@@ -1828,10 +1837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB03C53-D149-8D47-9F9C-2A5FA6F563CA}">
-  <dimension ref="A1:AB31"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -1853,10 +1862,10 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -1867,7 +1876,7 @@
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
       <c r="B2" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -1875,7 +1884,7 @@
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
       <c r="B3" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
@@ -1883,7 +1892,7 @@
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="26"/>
       <c r="B4" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -1915,13 +1924,13 @@
     </row>
     <row r="6" spans="1:28" s="2" customFormat="1" ht="127" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>29</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>9</v>
@@ -1936,10 +1945,10 @@
         <v>14</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J6" s="24" t="s">
         <v>1</v>
@@ -1951,16 +1960,16 @@
         <v>2</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N6" s="24" t="s">
         <v>3</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q6" s="23" t="s">
         <v>6</v>
@@ -1981,24 +1990,24 @@
         <v>11</v>
       </c>
       <c r="W6" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X6" s="23" t="s">
         <v>12</v>
       </c>
       <c r="Y6" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="45" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -2012,7 +2021,7 @@
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P7" s="18"/>
       <c r="Q7" s="6"/>
@@ -2034,13 +2043,13 @@
     </row>
     <row r="8" spans="1:28" ht="60" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="16" t="s">
@@ -2076,13 +2085,13 @@
     </row>
     <row r="9" spans="1:28" ht="52" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -2118,13 +2127,13 @@
     </row>
     <row r="10" spans="1:28" ht="43" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -2160,13 +2169,13 @@
     </row>
     <row r="11" spans="1:28" ht="65" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -2183,7 +2192,7 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q11" s="5" t="s">
         <v>6</v>
@@ -2202,13 +2211,13 @@
     </row>
     <row r="12" spans="1:28" ht="39" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -2244,13 +2253,13 @@
     </row>
     <row r="13" spans="1:28" ht="62" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -2258,7 +2267,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -2282,13 +2291,13 @@
     </row>
     <row r="14" spans="1:28" ht="58" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="16" t="s">
@@ -2323,97 +2332,89 @@
       </c>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" spans="1:28" ht="45" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>61</v>
-      </c>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
       <c r="B15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
+      <c r="N15" s="28"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
       <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="7">
-        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
-      </c>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="29"/>
+      <c r="AB15" s="20"/>
     </row>
-    <row r="16" spans="1:28" ht="65" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
+      <c r="S16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
       <c r="Y16" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="65" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -2425,17 +2426,15 @@
         <v>1</v>
       </c>
       <c r="K17" s="6"/>
-      <c r="L17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
       <c r="Q17" s="6"/>
-      <c r="R17" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
@@ -2444,23 +2443,21 @@
       <c r="X17" s="6"/>
       <c r="Y17" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="65" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="16" t="s">
-        <v>10</v>
-      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -2468,16 +2465,18 @@
       <c r="J18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="5"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
+      <c r="R18" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
@@ -2489,24 +2488,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="62" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="65" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="J19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
@@ -2518,91 +2523,85 @@
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
-      <c r="W19" s="16" t="s">
-        <v>69</v>
-      </c>
+      <c r="W19" s="6"/>
       <c r="X19" s="6"/>
       <c r="Y19" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="52" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" ht="62" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
-      <c r="U20" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="U20" s="6"/>
       <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
+      <c r="W20" s="16" t="s">
+        <v>68</v>
+      </c>
       <c r="X20" s="6"/>
       <c r="Y20" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="97" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>61</v>
+    <row r="21" spans="1:25" ht="52" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="5"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="L21" s="6"/>
-      <c r="M21" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
-      <c r="S21" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="S21" s="6"/>
       <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
+      <c r="U21" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
@@ -2611,38 +2610,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="52" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" ht="97" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>9</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
+      <c r="S22" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
@@ -2653,36 +2652,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="65" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>61</v>
+    <row r="23" spans="1:25" ht="52" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D23" s="16" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="6"/>
-      <c r="F23" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" s="5"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
-      <c r="Q23" s="5"/>
+      <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
@@ -2695,17 +2694,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="60" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" ht="65" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="E24" s="6"/>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -2713,18 +2714,16 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="J24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
-      <c r="Q24" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="Q24" s="5"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
@@ -2737,68 +2736,66 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="58" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" ht="60" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="K25" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
+      <c r="Q25" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="R25" s="6"/>
-      <c r="S25" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="S25" s="6"/>
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
-      <c r="X25" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="X25" s="6"/>
       <c r="Y25" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" ht="58" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="F26" s="6"/>
-      <c r="G26" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
@@ -2808,35 +2805,41 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
+      <c r="S26" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="T26" s="6"/>
-      <c r="U26" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="U26" s="6"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
+      <c r="X26" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="Y26" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" ht="45" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="G27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
@@ -2846,41 +2849,37 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
-      <c r="S27" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="S27" s="6"/>
       <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
+      <c r="U27" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
       <c r="Y27" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="58" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" ht="39" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="16" t="s">
-        <v>10</v>
-      </c>
+      <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
@@ -2888,37 +2887,41 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
+      <c r="S28" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="T28" s="6"/>
       <c r="U28" s="6"/>
-      <c r="V28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="W28" s="5"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
       <c r="X28" s="6"/>
       <c r="Y28" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" ht="58" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="E29" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
@@ -2926,26 +2929,29 @@
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
-      <c r="S29" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="U29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="W29" s="5"/>
       <c r="X29" s="6"/>
       <c r="Y29" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="C30" s="4"/>
+    <row r="30" spans="1:25" ht="39" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -2961,101 +2967,136 @@
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="5"/>
+      <c r="S30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="U30" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
       <c r="X30" s="6"/>
-      <c r="Y30" s="7"/>
+      <c r="Y30" s="7">
+        <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="31" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15">
-        <f>COUNTIF(A7:A29,"✓")/COUNTA(B7:B29)</f>
-        <v>1</v>
-      </c>
-      <c r="D31" s="11">
-        <f t="shared" ref="D31:R31" si="0">COUNTA(D7:D30)</f>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="7"/>
+    </row>
+    <row r="32" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
+        <f>COUNTIF(A7:A30,"✓")/COUNTA(B7:B30)</f>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D32" s="11">
+        <f t="shared" ref="D32:R32" si="0">COUNTA(D7:D31)</f>
         <v>4</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E32" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F32" s="11">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G32" s="11">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H32" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11">
+      <c r="I32" s="11"/>
+      <c r="J32" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K32" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L32" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M31" s="11">
+      <c r="M32" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N31" s="11">
+      <c r="N32" s="11">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="O31" s="11">
+      <c r="O32" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P31" s="11">
-        <f>COUNTA(P7:P30)</f>
+      <c r="P32" s="11">
+        <f>COUNTA(P7:P31)</f>
         <v>1</v>
       </c>
-      <c r="Q31" s="11">
+      <c r="Q32" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R32" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="S31" s="11">
-        <f t="shared" ref="S31" si="1">COUNTA(S7:S30)</f>
+      <c r="S32" s="11">
+        <f t="shared" ref="S32" si="1">COUNTA(S7:S31)</f>
         <v>7</v>
       </c>
-      <c r="T31" s="11">
-        <f>COUNTA(T7:T30)</f>
+      <c r="T32" s="11">
+        <f>COUNTA(T7:T31)</f>
         <v>5</v>
       </c>
-      <c r="U31" s="11">
-        <f>COUNTA(U7:U30)</f>
+      <c r="U32" s="11">
+        <f>COUNTA(U7:U31)</f>
         <v>5</v>
       </c>
-      <c r="V31" s="11">
-        <f>COUNTA(V7:V30)</f>
+      <c r="V32" s="11">
+        <f>COUNTA(V7:V31)</f>
         <v>2</v>
       </c>
-      <c r="W31" s="11">
-        <f>COUNTA(W7:W30)</f>
+      <c r="W32" s="11">
+        <f>COUNTA(W7:W31)</f>
         <v>1</v>
       </c>
-      <c r="X31" s="11">
-        <f>COUNTA(X7:X30)</f>
+      <c r="X32" s="11">
+        <f>COUNTA(X7:X31)</f>
         <v>2</v>
       </c>
-      <c r="Y31" s="13">
+      <c r="Y32" s="13">
         <f>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</f>
         <v>61</v>
       </c>
@@ -3069,7 +3110,7 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D31:X31">
+  <conditionalFormatting sqref="D32:X32">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3079,7 +3120,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y7:Y30">
+  <conditionalFormatting sqref="Y7:Y31">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
New expertise tag: "Nature"
</commit_message>
<xml_diff>
--- a/JSON/fgDeGender_Trefwoorden.xlsx
+++ b/JSON/fgDeGender_Trefwoorden.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD475C1E-EC5C-BF4E-B9AF-A403B711D102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35A056A-3C99-4744-B56A-605E3F663D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="26220" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
+    <workbookView xWindow="11660" yWindow="620" windowWidth="39540" windowHeight="26220" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabel" sheetId="1" r:id="rId1"/>
+    <sheet name="Bar chart" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="80">
   <si>
     <t>Albert</t>
   </si>
@@ -233,9 +234,6 @@
     <t xml:space="preserve">    ‣ Door Peter ingevulde trefwoorden mag je gerust aanpassen</t>
   </si>
   <si>
-    <t xml:space="preserve">    ‣ Je mag een ontbrekend trefwoord voorstellen (vaak leverbaar ;-)</t>
-  </si>
-  <si>
     <t>Museum</t>
   </si>
   <si>
@@ -245,9 +243,6 @@
     <t>Zelfexpressie</t>
   </si>
   <si>
-    <t>Mixed-Media</t>
-  </si>
-  <si>
     <t>Meervoudige-Belichting</t>
   </si>
   <si>
@@ -264,6 +259,24 @@
   </si>
   <si>
     <t>Vervloed</t>
+  </si>
+  <si>
+    <t>Gemengde technieken</t>
+  </si>
+  <si>
+    <t>Documentair</t>
+  </si>
+  <si>
+    <t>Industrieel erfgoed</t>
+  </si>
+  <si>
+    <t>Theater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ‣ Je mag een ontbrekend trefwoord voorstellen (er wordt iedere maand 1 nieuw trefwoord toegevoegd ;-)</t>
+  </si>
+  <si>
+    <t>Natuur</t>
   </si>
 </sst>
 </file>
@@ -273,7 +286,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -357,8 +370,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +393,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,9 +451,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
@@ -454,26 +476,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="59">
     <dxf>
       <font>
         <b val="0"/>
@@ -886,6 +909,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -903,6 +927,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -920,7 +945,65 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -959,7 +1042,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -995,11 +1078,11 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1013,11 +1096,11 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1031,7 +1114,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1049,7 +1132,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1067,7 +1150,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1085,7 +1168,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1139,7 +1222,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1175,7 +1258,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1193,7 +1276,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1211,7 +1294,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1265,7 +1348,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1283,7 +1366,7 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1301,7 +1384,61 @@
         <name val="Aptos Narrow"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1441,77 +1578,1950 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{07BF255B-9F3C-F444-B242-BB5A274F9C2E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000018-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FFDA7056-77C5-0E45-B228-FAA030B13D3D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000019-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{838CB56F-750F-CF4D-A526-F8BDD6153893}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001A-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B5EAD0E9-0CB7-7643-BBF6-515D41DE2AB9}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001B-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{80CEE508-BFBF-8B41-9B2E-1D71B70E916B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001C-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{615328DC-C8C5-354D-9B63-3814CA00AC4E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001D-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C4E7032B-BA3D-4843-A507-EC6FA76C7065}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001E-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0EC6D8B2-C0AF-974A-A78A-CCFFB3DE3323}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001F-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E3A7FB54-58C4-8E41-A14E-91D9B4D2A5D7}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000020-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{87E90FB9-046D-C944-8DA5-E139BDA219D6}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000021-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{CAB07FF6-BB60-054A-8EBB-886F936878DB}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000022-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{EE74B8EA-88C3-5344-973D-E78682161304}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000023-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A5BD1A33-37EB-0847-A6EF-CD504040852A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000024-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1C10049A-74B5-F24D-9812-99F45D05156C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000025-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6CD2A583-6522-7343-B22C-C17005E023A4}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000026-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A6318B4F-D2EB-C349-942D-52A38B78BDD5}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000027-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FCC83C24-FE1C-1949-9ABE-A44360C0C79A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000028-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{01C8C26C-ECDE-294D-9D80-F2EC33FF8124}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000029-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{65D964F9-50E1-0444-AC83-2EF9F4907A97}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002A-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{5C7DEEE3-09CE-E846-8554-1240043D94B5}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002B-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D5ACF4A5-8741-AB4E-B526-BD62E1F98325}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002C-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E8D3986C-5C2A-DB4C-ACBC-F7D2146B10F5}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002D-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{26590BB9-0434-2147-8023-7D54CB30F425}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002E-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AFA216D4-A56B-F34B-816E-E23F291E117D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>, </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002F-0556-3D42-A119-493FF768DFA4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="0">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:separator>, </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Bar chart'!$D$31:$AA$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabel!$D$32:$AA$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="cylinder"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Tabel!$D$31:$AA$31</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="24"/>
+                  <c:pt idx="0">
+                    <c:v>Abstract</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Architectuur</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Conceptueel</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Concert</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Documentair</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Drone</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Experimenteel</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Gemengde technieken</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Industrieel erfgoed</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Landschap</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Macro</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Meervoudige-Belichting</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minimaal</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Museum</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Nabewerking</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Natuur</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Panorama</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Portret</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Straat</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>Reis</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>Theater</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>Vogels</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>Zelfexpressie</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>Zwart-wit</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0556-3D42-A119-493FF768DFA4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="1442005888"/>
+        <c:axId val="1442019328"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1442005888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1442019328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1442019328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1442005888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F864821-DB4F-FE45-B959-579C992F4BC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:Y32" totalsRowCount="1" headerRowDxfId="52" dataDxfId="51" totalsRowDxfId="50">
-  <autoFilter ref="A6:Y31" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
-  <tableColumns count="25">
-    <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}" name="Table1" displayName="Table1" ref="A6:AB32" totalsRowCount="1" headerRowDxfId="58" dataDxfId="57" totalsRowDxfId="56">
+  <autoFilter ref="A6:AB31" xr:uid="{18A14CD0-18C7-B54E-BC1D-313A04F7E9E7}"/>
+  <tableColumns count="28">
+    <tableColumn id="19" xr3:uid="{2104FAC0-B37F-7E4D-8035-A0C747D5CE8A}" name="Gezien?" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="27">
       <totalsRowFormula>COUNTIF(A7:A30,"✓")/COUNTA(B7:B30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="48" totalsRowDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="47" totalsRowDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{3B6A13EE-99F5-7441-8057-E1A06F70075A}" name="Abstract" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="21">
-      <totalsRowFormula>COUNTA(D7:D31)</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{9313EFF0-1C40-7F4D-B439-C13034C06AA1}" name="voornaam" dataDxfId="54" totalsRowDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{FE987FD6-D8D1-0F4A-A4B4-1E737B6E77DF}" name="achternaam" dataDxfId="53" totalsRowDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{3B6A13EE-99F5-7441-8057-E1A06F70075A}" name="Abstract" totalsRowFunction="custom" dataDxfId="52" totalsRowDxfId="24">
+      <totalsRowFormula>COUNTA(D7:D30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E9B92604-5273-624A-92B0-22FFB11BEC40}" name="Architectuur" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="20">
-      <totalsRowFormula>COUNTA(E7:E31)</totalsRowFormula>
+    <tableColumn id="4" xr3:uid="{E9B92604-5273-624A-92B0-22FFB11BEC40}" name="Architectuur" totalsRowFunction="custom" dataDxfId="51" totalsRowDxfId="23">
+      <totalsRowFormula>COUNTA(E7:E30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{832AF978-DCE3-DA47-B36A-9D928FCF0BF1}" name="Conceptueel" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="19">
-      <totalsRowFormula>COUNTA(F7:F31)</totalsRowFormula>
+    <tableColumn id="6" xr3:uid="{832AF978-DCE3-DA47-B36A-9D928FCF0BF1}" name="Conceptueel" totalsRowFunction="custom" dataDxfId="50" totalsRowDxfId="22">
+      <totalsRowFormula>COUNTA(F7:F30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64143930-3345-DA4D-9135-20E16BCCB08E}" name="Concert" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="18">
-      <totalsRowFormula>COUNTA(G7:G31)</totalsRowFormula>
+    <tableColumn id="7" xr3:uid="{64143930-3345-DA4D-9135-20E16BCCB08E}" name="Concert" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="21">
+      <totalsRowFormula>COUNTA(G7:G30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{32897D46-8F9F-3E49-B198-8C097B1CCB00}" name="Drone" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="17">
-      <totalsRowFormula>COUNTA(H7:H31)</totalsRowFormula>
+    <tableColumn id="18" xr3:uid="{E9A6A14D-691C-F049-BD47-F88709944822}" name="Documentair" totalsRowFunction="custom" dataDxfId="48" totalsRowDxfId="20">
+      <totalsRowFormula>COUNTA(H7:H30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{E9A6A14D-691C-F049-BD47-F88709944822}" name="Documentary" dataDxfId="41" totalsRowDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="15">
-      <totalsRowFormula>COUNTA(J7:J31)</totalsRowFormula>
+    <tableColumn id="28" xr3:uid="{26BA5735-8FA4-1B47-ADDD-51B9B173A24B}" name="Drone" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="19">
+      <totalsRowFormula>COUNTA(I7:I30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="14">
-      <totalsRowFormula>COUNTA(K7:K31)</totalsRowFormula>
+    <tableColumn id="8" xr3:uid="{6A3F59BA-3F98-6A4B-A8C1-EA8AB1DE8931}" name="Experimenteel" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="18">
+      <totalsRowFormula>COUNTA(J7:J30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="13">
-      <totalsRowFormula>COUNTA(L7:L31)</totalsRowFormula>
+    <tableColumn id="24" xr3:uid="{BD4AC84F-7EFF-4D44-8D7A-3269773F41AC}" name="Gemengde technieken" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="17">
+      <totalsRowFormula>COUNTA(K7:K30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{2E8FBDE5-5DE6-8F45-9CD3-D96DE8979E6D}" name="Meervoudige-Belichting" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="12">
-      <totalsRowFormula>COUNTA(M7:M31)</totalsRowFormula>
+    <tableColumn id="29" xr3:uid="{51AA6F9C-A86D-4641-89DA-9684F3AB0BEB}" name="Industrieel erfgoed" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="16">
+      <totalsRowFormula>COUNTA(L7:L30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="11">
-      <totalsRowFormula>COUNTA(N7:N31)</totalsRowFormula>
+    <tableColumn id="9" xr3:uid="{9808A521-A328-EE4B-B306-58401B0D19E2}" name="Landschap" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="15">
+      <totalsRowFormula>COUNTA(M7:M30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{34A8085A-25B7-B64C-9185-7DCD6F2A68CF}" name="Museum" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="10">
-      <totalsRowFormula>COUNTA(O7:O31)</totalsRowFormula>
+    <tableColumn id="10" xr3:uid="{6294B401-5148-FB4A-BB17-7323DF030296}" name="Macro" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="14">
+      <totalsRowFormula>COUNTA(N7:N30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{5B57471E-1B52-2048-A846-292B312EF0C6}" name="Mixed-Media" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="9">
-      <totalsRowFormula>COUNTA(P7:P31)</totalsRowFormula>
+    <tableColumn id="25" xr3:uid="{2E8FBDE5-5DE6-8F45-9CD3-D96DE8979E6D}" name="Meervoudige-Belichting" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="13">
+      <totalsRowFormula>COUNTA(O7:O30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="8">
-      <totalsRowFormula>COUNTA(Q7:Q31)</totalsRowFormula>
+    <tableColumn id="11" xr3:uid="{1D8616D1-F1AE-AE48-AFB2-A7D87E1157ED}" name="Minimaal" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="12">
+      <totalsRowFormula>COUNTA(P7:P30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="7">
-      <totalsRowFormula>COUNTA(R7:R31)</totalsRowFormula>
+    <tableColumn id="5" xr3:uid="{34A8085A-25B7-B64C-9185-7DCD6F2A68CF}" name="Museum" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="11">
+      <totalsRowFormula>COUNTA(Q7:Q30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="6">
-      <totalsRowFormula>COUNTA(S7:S31)</totalsRowFormula>
+    <tableColumn id="12" xr3:uid="{093E5B61-D203-5D46-A11D-0D0EADE5D84D}" name="Nabewerking" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="10">
+      <totalsRowFormula>COUNTA(R7:R30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="5">
-      <totalsRowFormula>COUNTA(T7:T31)</totalsRowFormula>
+    <tableColumn id="31" xr3:uid="{15E36B58-C01C-FB4B-B5D8-EEA6781A51BE}" name="Natuur" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="9">
+      <totalsRowFormula>COUNTA(S7:S30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="4">
-      <totalsRowFormula>COUNTA(U7:U31)</totalsRowFormula>
+    <tableColumn id="13" xr3:uid="{1B1A8610-E3F0-BB41-8404-F7FBFBFD2F46}" name="Panorama" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="8">
+      <totalsRowFormula>COUNTA(T7:T30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="3">
-      <totalsRowFormula>COUNTA(V7:V31)</totalsRowFormula>
+    <tableColumn id="14" xr3:uid="{7BE0DD55-472B-A749-A072-3480901CD6EE}" name="Portret" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="7">
+      <totalsRowFormula>COUNTA(U7:U30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{0BCDD0DC-39BA-EE43-BE8C-DB82549B10E5}" name="Zelfexpressie" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="2">
-      <totalsRowFormula>COUNTA(W7:W31)</totalsRowFormula>
+    <tableColumn id="15" xr3:uid="{E2F14896-3DF7-4F48-ACE8-62674FA0BC06}" name="Straat" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="6">
+      <totalsRowFormula>COUNTA(V7:V30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="1">
-      <totalsRowFormula>COUNTA(X7:X31)</totalsRowFormula>
+    <tableColumn id="16" xr3:uid="{65AC9D6E-D00B-A44E-9C3A-14BE8992B6DC}" name="Reis" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="5">
+      <totalsRowFormula>COUNTA(W7:W30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#/persoon" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="0">
+    <tableColumn id="30" xr3:uid="{AAC74AD1-DFCE-8D42-A34A-0FF047CE9A9B}" name="Theater" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="4">
+      <totalsRowFormula>COUNTA(X7:X30)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="21" xr3:uid="{4AEC1E64-2A6A-B448-B282-9243A0CD40E2}" name="Vogels" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="3">
+      <totalsRowFormula>COUNTA(Y7:Y30)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="20" xr3:uid="{0BCDD0DC-39BA-EE43-BE8C-DB82549B10E5}" name="Zelfexpressie" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="2">
+      <totalsRowFormula>COUNTA(Z7:Z30)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{7F963F99-D388-E245-AA46-94693F4DD104}" name="Zwart-wit" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="1">
+      <totalsRowFormula>COUNTA(AA7:AA30)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{2371FB57-2F1C-D847-A09F-99790B0E7E04}" name="#/persoon" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="0">
       <calculatedColumnFormula>COUNTA(#REF!)</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</totalsRowFormula>
     </tableColumn>
@@ -1837,10 +3847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB03C53-D149-8D47-9F9C-2A5FA6F563CA}">
-  <dimension ref="A1:AB32"/>
+  <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -1850,156 +3860,168 @@
     <col min="3" max="3" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="11" width="10.83203125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="1"/>
-    <col min="14" max="18" width="10.83203125" style="1" customWidth="1"/>
-    <col min="19" max="21" width="10.83203125" style="1"/>
-    <col min="22" max="23" width="13.83203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" style="1"/>
-    <col min="25" max="25" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="13" width="10.83203125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="10.83203125" style="1"/>
+    <col min="16" max="20" width="10.83203125" style="1" customWidth="1"/>
+    <col min="21" max="24" width="10.83203125" style="1"/>
+    <col min="25" max="26" width="13.83203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="10.83203125" style="1"/>
+    <col min="28" max="28" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="AB1" s="14">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" s="28"/>
+      <c r="B2" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" s="28"/>
+      <c r="B4" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="18"/>
+    </row>
+    <row r="6" spans="1:31" s="2" customFormat="1" ht="127" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="Y1" s="14">
-        <v>45789</v>
+      <c r="L6" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="R6" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="T6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="W6" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="X6" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z6" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA6" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB6" s="23" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="19"/>
-    </row>
-    <row r="6" spans="1:28" s="2" customFormat="1" ht="127" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="N6" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q6" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="R6" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="S6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="T6" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="U6" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="V6" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="W6" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="X6" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y6" s="24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" ht="45" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>60</v>
       </c>
@@ -2007,7 +4029,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -2020,28 +4042,29 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
-      <c r="O7" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="17" t="s">
+        <v>65</v>
+      </c>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
-      <c r="T7" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="U7" s="17" t="s">
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="7">
+      <c r="X7" s="16"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" ht="30" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>60</v>
       </c>
@@ -2052,9 +4075,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="16" t="s">
-        <v>10</v>
-      </c>
+      <c r="E8" s="15"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -2066,24 +4087,25 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
-      <c r="Q8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
       <c r="T8" s="6"/>
-      <c r="U8" s="5" t="s">
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="7">
+      <c r="X8" s="5"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="52" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" ht="52" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>60</v>
       </c>
@@ -2100,32 +4122,33 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
-      <c r="V9" s="5" t="s">
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W9" s="5"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="7">
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" ht="43" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>60</v>
       </c>
@@ -2138,11 +4161,11 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -2152,22 +4175,23 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
-      <c r="S10" s="5" t="s">
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
+      <c r="V10" s="5"/>
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
-      <c r="Y10" s="7">
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="65" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" ht="93" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>60</v>
       </c>
@@ -2186,30 +4210,31 @@
       <c r="J11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+      <c r="K11" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="15"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="5"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="6"/>
       <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
+      <c r="V11" s="5"/>
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
-      <c r="Y11" s="7">
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" ht="36" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>60</v>
       </c>
@@ -2227,31 +4252,30 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
-      <c r="S12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T12" s="5" t="s">
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
-      <c r="Y12" s="7">
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="62" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" ht="62" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>60</v>
       </c>
@@ -2265,10 +4289,10 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="H13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="5"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -2284,12 +4308,15 @@
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
-      <c r="Y13" s="7">
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="58" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" ht="58" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>60</v>
       </c>
@@ -2300,7 +4327,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="6"/>
@@ -2308,11 +4335,11 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -2323,48 +4350,54 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
-      <c r="X14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y14" s="7">
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
-      </c>
-      <c r="AB14" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="AE14" s="19"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
+        <v>73</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="28"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
       <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="29"/>
-      <c r="AB15" s="20"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="29">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="19"/>
     </row>
-    <row r="16" spans="1:28" ht="45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" ht="39" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>60</v>
       </c>
@@ -2374,9 +4407,7 @@
       <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>9</v>
-      </c>
+      <c r="D16" s="15"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -2391,22 +4422,25 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="5" t="s">
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T16" s="5" t="s">
+      <c r="V16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
-      <c r="Y16" s="7">
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="65" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="65" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>60</v>
       </c>
@@ -2425,15 +4459,15 @@
       <c r="J17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="6"/>
+      <c r="Q17" s="5"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
@@ -2441,12 +4475,15 @@
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
-      <c r="Y17" s="7">
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="65" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="50" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>60</v>
       </c>
@@ -2462,33 +4499,34 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="5" t="s">
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
+      <c r="O18" s="5"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
-      <c r="R18" s="5" t="s">
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
-      <c r="Y18" s="7">
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="65" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="65" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>60</v>
       </c>
@@ -2499,9 +4537,7 @@
         <v>37</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="16" t="s">
-        <v>10</v>
-      </c>
+      <c r="E19" s="15"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -2509,11 +4545,11 @@
       <c r="J19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
@@ -2525,12 +4561,15 @@
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
-      <c r="Y19" s="7">
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="62" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="62" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>60</v>
       </c>
@@ -2559,16 +4598,19 @@
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
-      <c r="W20" s="16" t="s">
-        <v>68</v>
-      </c>
+      <c r="W20" s="6"/>
       <c r="X20" s="6"/>
-      <c r="Y20" s="7">
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="52" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="47" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>60</v>
       </c>
@@ -2585,32 +4627,33 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="K21" s="6"/>
       <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="5" t="s">
+      <c r="M21" s="5"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="6"/>
+      <c r="Q21" s="5"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
-      <c r="U21" s="5" t="s">
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="7">
+      <c r="X21" s="5"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="97" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="97" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>60</v>
       </c>
@@ -2629,30 +4672,33 @@
       <c r="J22" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
+      <c r="O22" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
-      <c r="S22" s="5" t="s">
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
-      <c r="Y22" s="7">
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="52" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="45" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>60</v>
       </c>
@@ -2662,7 +4708,7 @@
       <c r="C23" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="6"/>
@@ -2671,15 +4717,13 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L23" s="5" t="s">
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M23" s="5"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+      <c r="O23" s="5"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
@@ -2689,12 +4733,15 @@
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
-      <c r="Y23" s="7">
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="65" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="59" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>60</v>
       </c>
@@ -2704,7 +4751,7 @@
       <c r="C24" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="6"/>
@@ -2714,29 +4761,30 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
-      <c r="Y24" s="7">
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="60" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" ht="59" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>60</v>
       </c>
@@ -2755,30 +4803,31 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
-      <c r="Q25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
-      <c r="Y25" s="7">
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="58" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="58" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>60</v>
       </c>
@@ -2789,7 +4838,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="6"/>
@@ -2805,22 +4854,23 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="S26" s="5" t="s">
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
-      <c r="X26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y26" s="7">
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" ht="45" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>60</v>
       </c>
@@ -2830,16 +4880,16 @@
       <c r="C27" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
@@ -2851,18 +4901,21 @@
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
-      <c r="U27" s="5" t="s">
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
-      <c r="Y27" s="7">
+      <c r="X27" s="5"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" ht="39" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>60</v>
       </c>
@@ -2887,20 +4940,25 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
-      <c r="S28" s="5" t="s">
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
       <c r="V28" s="6"/>
-      <c r="W28" s="6"/>
-      <c r="X28" s="6"/>
-      <c r="Y28" s="7">
+      <c r="W28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="58" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" ht="52" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>60</v>
       </c>
@@ -2911,19 +4969,17 @@
         <v>19</v>
       </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="16" t="s">
-        <v>10</v>
-      </c>
+      <c r="E29" s="15"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="5" t="s">
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
@@ -2932,17 +4988,20 @@
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
-      <c r="V29" s="5" t="s">
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W29" s="5"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="7">
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" ht="39" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>60</v>
       </c>
@@ -2959,159 +5018,248 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
-      <c r="S30" s="5" t="s">
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T30" s="5" t="s">
+      <c r="V30" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U30" s="5" t="s">
+      <c r="W30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="7">
+      <c r="X30" s="5"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="7">
         <f>COUNTA(Table1[[#This Row],[Abstract]:[Zwart-wit]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
-      <c r="Y31" s="7"/>
+      <c r="D31" s="6" t="str">
+        <f t="shared" ref="D31:AA31" si="0">D$6</f>
+        <v>Abstract</v>
+      </c>
+      <c r="E31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Architectuur</v>
+      </c>
+      <c r="F31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Conceptueel</v>
+      </c>
+      <c r="G31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Concert</v>
+      </c>
+      <c r="H31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Documentair</v>
+      </c>
+      <c r="I31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Drone</v>
+      </c>
+      <c r="J31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Experimenteel</v>
+      </c>
+      <c r="K31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Gemengde technieken</v>
+      </c>
+      <c r="L31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Industrieel erfgoed</v>
+      </c>
+      <c r="M31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Landschap</v>
+      </c>
+      <c r="N31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Macro</v>
+      </c>
+      <c r="O31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Meervoudige-Belichting</v>
+      </c>
+      <c r="P31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Minimaal</v>
+      </c>
+      <c r="Q31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Museum</v>
+      </c>
+      <c r="R31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Nabewerking</v>
+      </c>
+      <c r="S31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Natuur</v>
+      </c>
+      <c r="T31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Panorama</v>
+      </c>
+      <c r="U31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Portret</v>
+      </c>
+      <c r="V31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Straat</v>
+      </c>
+      <c r="W31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Reis</v>
+      </c>
+      <c r="X31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Theater</v>
+      </c>
+      <c r="Y31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Vogels</v>
+      </c>
+      <c r="Z31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Zelfexpressie</v>
+      </c>
+      <c r="AA31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Zwart-wit</v>
+      </c>
+      <c r="AB31" s="7"/>
     </row>
-    <row r="32" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15">
+    <row r="32" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26">
         <f>COUNTIF(A7:A30,"✓")/COUNTA(B7:B30)</f>
         <v>0.95833333333333337</v>
       </c>
       <c r="D32" s="11">
-        <f t="shared" ref="D32:R32" si="0">COUNTA(D7:D31)</f>
+        <f t="shared" ref="D32:AA32" si="1">COUNTA(D7:D30)</f>
+        <v>3</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F32" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G32" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H32" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I32" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="11">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E32" s="11">
-        <f t="shared" si="0"/>
+      <c r="K32" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L32" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="11">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F32" s="11">
-        <f t="shared" si="0"/>
+      <c r="N32" s="11">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G32" s="11">
-        <f t="shared" si="0"/>
+      <c r="O32" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P32" s="11">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H32" s="11">
-        <f t="shared" si="0"/>
+      <c r="Q32" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R32" s="11">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11">
-        <f t="shared" si="0"/>
+      <c r="S32" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T32" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U32" s="11">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K32" s="11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="L32" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M32" s="11">
-        <f t="shared" si="0"/>
+      <c r="V32" s="11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="W32" s="11">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="X32" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y32" s="11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Z32" s="11">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N32" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="O32" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P32" s="11">
-        <f>COUNTA(P7:P31)</f>
-        <v>1</v>
-      </c>
-      <c r="Q32" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R32" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S32" s="11">
-        <f t="shared" ref="S32" si="1">COUNTA(S7:S31)</f>
-        <v>7</v>
-      </c>
-      <c r="T32" s="11">
-        <f>COUNTA(T7:T31)</f>
-        <v>5</v>
-      </c>
-      <c r="U32" s="11">
-        <f>COUNTA(U7:U31)</f>
-        <v>5</v>
-      </c>
-      <c r="V32" s="11">
-        <f>COUNTA(V7:V31)</f>
-        <v>2</v>
-      </c>
-      <c r="W32" s="11">
-        <f>COUNTA(W7:W31)</f>
-        <v>1</v>
-      </c>
-      <c r="X32" s="11">
-        <f>COUNTA(X7:X31)</f>
-        <v>2</v>
-      </c>
-      <c r="Y32" s="13">
+      <c r="AA32" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="13">
         <f>SUM(Table1[[#Totals],[Abstract]:[Zwart-wit]])</f>
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A5:V5"/>
+  <mergeCells count="2">
+    <mergeCell ref="A5:Y5"/>
     <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D32:X32">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="D32:AA32">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3120,7 +5268,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y7:Y31">
+  <conditionalFormatting sqref="AB7:AB31">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3146,4 +5294,19 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B97817-31CE-4A41-AB90-38A9CE04187E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>